<commit_message>
Added JS220 Safety Banana Jack front panel.
Fixed connector part numbers for BOM.
</commit_message>
<xml_diff>
--- a/eagle/fp_safety_banana/js220_fp_sba_bom.xlsx
+++ b/eagle/fp_safety_banana/js220_fp_sba_bom.xlsx
@@ -600,7 +600,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>2024 October 14</t>
+          <t>2024 October 29</t>
         </is>
       </c>
     </row>
@@ -640,7 +640,7 @@
       </c>
       <c r="D5" s="9" t="inlineStr">
         <is>
-          <t>CT3151V1-0</t>
+          <t>CT3149-0</t>
         </is>
       </c>
     </row>
@@ -658,7 +658,7 @@
       </c>
       <c r="D6" s="9" t="inlineStr">
         <is>
-          <t>CT3151V1-2</t>
+          <t>CT3149-2</t>
         </is>
       </c>
     </row>
@@ -676,7 +676,7 @@
       </c>
       <c r="D7" s="9" t="inlineStr">
         <is>
-          <t>CT3151V1-4</t>
+          <t>CT3149-4</t>
         </is>
       </c>
     </row>
@@ -761,7 +761,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>2024 October 14</t>
+          <t>2024 October 29</t>
         </is>
       </c>
     </row>
@@ -801,7 +801,7 @@
       </c>
       <c r="D5" s="9" t="inlineStr">
         <is>
-          <t>CT3151V1-0</t>
+          <t>CT3149-0</t>
         </is>
       </c>
     </row>
@@ -819,7 +819,7 @@
       </c>
       <c r="D6" s="9" t="inlineStr">
         <is>
-          <t>CT3151V1-2</t>
+          <t>CT3149-2</t>
         </is>
       </c>
     </row>
@@ -837,7 +837,7 @@
       </c>
       <c r="D7" s="9" t="inlineStr">
         <is>
-          <t>CT3151V1-4</t>
+          <t>CT3149-4</t>
         </is>
       </c>
     </row>
@@ -922,7 +922,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>2024 October 14</t>
+          <t>2024 October 29</t>
         </is>
       </c>
     </row>

</xml_diff>